<commit_message>
Fitur Product & Kategori Admin
</commit_message>
<xml_diff>
--- a/database/FileExcel/Category.xlsx
+++ b/database/FileExcel/Category.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yovie\persediaanapp-magang\database\FileExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DCEDB2-6E60-4638-B1F3-05CCFC7798E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E543F8E-8915-479E-B4D2-A86B29F86607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="450" windowWidth="6670" windowHeight="10080" xr2:uid="{B1A6D6DA-43F5-4D03-876B-1BE0E6BF7134}"/>
+    <workbookView xWindow="8130" yWindow="600" windowWidth="6670" windowHeight="10080" xr2:uid="{B1A6D6DA-43F5-4D03-876B-1BE0E6BF7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -84,6 +83,9 @@
   </si>
   <si>
     <t>aksesoris</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -452,15 +454,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC210C0-9D73-46BA-9C56-AD0FD5D86CE8}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,13 +473,16 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
@@ -487,11 +492,14 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="K2" s="2"/>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1"/>
       <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>2</v>
       </c>
@@ -501,9 +509,12 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>3</v>
       </c>
@@ -513,8 +524,11 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>4</v>
       </c>
@@ -524,8 +538,11 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>5</v>
       </c>
@@ -535,8 +552,11 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>6</v>
       </c>
@@ -545,6 +565,9 @@
       </c>
       <c r="C7" t="s">
         <v>16</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>